<commit_message>
find_home to rent_home & buy_home put in entities.HomeOwner()
</commit_message>
<xml_diff>
--- a/inputs/desaster_input_data_template.xlsx
+++ b/inputs/desaster_input_data_template.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="79">
   <si>
     <t>Savings</t>
   </si>
@@ -249,6 +249,24 @@
   </si>
   <si>
     <t>Owner Occupied</t>
+  </si>
+  <si>
+    <t>341 Where St</t>
+  </si>
+  <si>
+    <t>Gal</t>
+  </si>
+  <si>
+    <t>For Alfred</t>
+  </si>
+  <si>
+    <t>For Selena</t>
+  </si>
+  <si>
+    <t>9900 Nowhere St</t>
+  </si>
+  <si>
+    <t>Blake</t>
   </si>
 </sst>
 </file>
@@ -304,19 +322,281 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="38" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="38" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="133">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -592,10 +872,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V9"/>
+  <dimension ref="A1:V11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1235,8 +1515,147 @@
         <v>700</v>
       </c>
     </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
+        <v>71</v>
+      </c>
+      <c r="E10">
+        <v>60000</v>
+      </c>
+      <c r="F10">
+        <v>1000</v>
+      </c>
+      <c r="G10">
+        <v>700</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10" s="2">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>1100</v>
+      </c>
+      <c r="M10">
+        <v>1920</v>
+      </c>
+      <c r="N10">
+        <f>L10*279</f>
+        <v>306900</v>
+      </c>
+      <c r="O10" t="s">
+        <v>67</v>
+      </c>
+      <c r="P10" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q10">
+        <v>30000</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10" t="b">
+        <v>1</v>
+      </c>
+      <c r="T10">
+        <v>-90.294238000000007</v>
+      </c>
+      <c r="U10">
+        <v>43.224015000000001</v>
+      </c>
+      <c r="V10">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E11" s="3">
+        <v>60000</v>
+      </c>
+      <c r="F11" s="3">
+        <v>1000</v>
+      </c>
+      <c r="G11" s="3">
+        <v>700</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0</v>
+      </c>
+      <c r="I11" s="4">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>2</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>750</v>
+      </c>
+      <c r="M11">
+        <v>1960</v>
+      </c>
+      <c r="N11">
+        <f t="shared" ref="N11" si="5">L11*279</f>
+        <v>209250</v>
+      </c>
+      <c r="O11" t="s">
+        <v>67</v>
+      </c>
+      <c r="P11" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q11" s="3">
+        <v>30000</v>
+      </c>
+      <c r="R11" s="3">
+        <v>0</v>
+      </c>
+      <c r="S11" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="T11" s="3">
+        <v>-90.294238000000007</v>
+      </c>
+      <c r="U11" s="3">
+        <v>43.224015000000001</v>
+      </c>
+      <c r="V11" s="3">
+        <v>700</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -1245,7 +1664,7 @@
   <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1317,7 +1736,7 @@
         <v>60000</v>
       </c>
       <c r="C2">
-        <v>100</v>
+        <v>100000</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1410,7 +1829,7 @@
         <v>837000</v>
       </c>
       <c r="N3" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="O3" t="b">
         <v>0</v>
@@ -1433,7 +1852,7 @@
         <v>45000</v>
       </c>
       <c r="C4">
-        <v>100</v>
+        <v>50000</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -1526,7 +1945,7 @@
         <v>558000</v>
       </c>
       <c r="N5" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="O5" t="b">
         <v>0</v>
@@ -1673,7 +2092,7 @@
       </c>
       <c r="F8" s="2">
         <f t="shared" si="0"/>
-        <v>1449.4183821327754</v>
+        <v>1010.9693215376109</v>
       </c>
       <c r="G8" t="s">
         <v>15</v>
@@ -1694,7 +2113,8 @@
         <v>1960</v>
       </c>
       <c r="M8">
-        <v>300000</v>
+        <f t="shared" ref="M8" si="2">K8*279</f>
+        <v>209250</v>
       </c>
       <c r="N8" t="s">
         <v>67</v>
@@ -1771,6 +2191,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Attempting to get renter and landlord processes in parallel
</commit_message>
<xml_diff>
--- a/inputs/desaster_input_data_template.xlsx
+++ b/inputs/desaster_input_data_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="renters" sheetId="5" r:id="rId1"/>
@@ -322,8 +322,38 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="133">
+  <cellStyleXfs count="163">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -464,7 +494,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="38" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="133">
+  <cellStyles count="163">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -531,6 +561,21 @@
     <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -597,6 +642,21 @@
     <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -874,8 +934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1107,11 +1167,10 @@
         <v>71</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
-        <v>59520</v>
+        <v>1000000</v>
       </c>
       <c r="F4">
-        <v>1000</v>
+        <v>1000000</v>
       </c>
       <c r="G4">
         <v>700</v>
@@ -1663,8 +1722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Changes to rent_home & buy_home for sheltering; .occupy() to .occupy_permanent()
</commit_message>
<xml_diff>
--- a/inputs/desaster_input_data_template.xlsx
+++ b/inputs/desaster_input_data_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="renters" sheetId="5" r:id="rId1"/>
@@ -305,12 +305,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -322,7 +328,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="163">
+  <cellStyleXfs count="173">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -486,15 +492,29 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="38" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="38" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="38" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="163">
+  <cellStyles count="173">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -576,6 +596,11 @@
     <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -657,6 +682,11 @@
     <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -934,8 +964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1223,74 +1253,74 @@
         <v>700</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="8">
         <f t="shared" si="0"/>
         <v>238080</v>
       </c>
-      <c r="F5">
-        <v>1000</v>
-      </c>
-      <c r="G5">
-        <v>700</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
+      <c r="F5" s="8">
+        <v>1000000</v>
+      </c>
+      <c r="G5" s="8">
+        <v>700</v>
+      </c>
+      <c r="H5" s="8">
+        <v>0</v>
+      </c>
+      <c r="I5" s="8">
         <f t="shared" si="1"/>
         <v>4960</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="8">
         <v>2</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="8">
         <v>2</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="8">
         <v>2000</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="8">
         <v>2010</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="8">
         <f t="shared" si="2"/>
         <v>558000</v>
       </c>
-      <c r="O5" t="s">
+      <c r="O5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="P5" t="s">
+      <c r="P5" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="Q5">
+      <c r="Q5" s="8">
         <v>30000</v>
       </c>
-      <c r="R5">
-        <v>1</v>
-      </c>
-      <c r="S5" t="b">
-        <v>0</v>
-      </c>
-      <c r="T5">
+      <c r="R5" s="8">
+        <v>1</v>
+      </c>
+      <c r="S5" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="T5" s="8">
         <v>-90.293058000000002</v>
       </c>
-      <c r="U5">
+      <c r="U5" s="8">
         <v>43.223936999999999</v>
       </c>
-      <c r="V5">
+      <c r="V5" s="8">
         <v>700</v>
       </c>
     </row>
@@ -1504,73 +1534,73 @@
         <v>700</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="9" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="8">
         <v>100000000</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="8">
         <v>1000</v>
       </c>
-      <c r="G9">
-        <v>700</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
+      <c r="G9" s="8">
+        <v>700</v>
+      </c>
+      <c r="H9" s="8">
+        <v>0</v>
+      </c>
+      <c r="I9" s="8">
         <f t="shared" si="3"/>
         <v>4960</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="8">
         <v>2</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="8">
         <v>2</v>
       </c>
-      <c r="L9">
+      <c r="L9" s="8">
         <v>2000</v>
       </c>
-      <c r="M9">
+      <c r="M9" s="8">
         <v>2010</v>
       </c>
-      <c r="N9">
+      <c r="N9" s="8">
         <f t="shared" si="4"/>
         <v>558000</v>
       </c>
-      <c r="O9" t="s">
+      <c r="O9" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="P9" t="s">
+      <c r="P9" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="Q9">
+      <c r="Q9" s="8">
         <v>100000000</v>
       </c>
-      <c r="R9">
-        <v>1</v>
-      </c>
-      <c r="S9" t="b">
-        <v>1</v>
-      </c>
-      <c r="T9">
+      <c r="R9" s="8">
+        <v>1</v>
+      </c>
+      <c r="S9" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="T9" s="8">
         <v>-90.295739999999995</v>
       </c>
-      <c r="U9">
+      <c r="U9" s="8">
         <v>43.223359000000002</v>
       </c>
-      <c r="V9">
+      <c r="V9" s="8">
         <v>700</v>
       </c>
     </row>
@@ -1722,8 +1752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1787,61 +1817,61 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="5">
         <v>60000</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="5">
         <v>100000</v>
       </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D2" s="5">
+        <v>0</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="6">
         <f>-PMT(0.05/12,360,(M2-M2*0.1),0)</f>
         <v>1482.7550049218294</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2">
+      <c r="I2" s="5">
+        <v>1</v>
+      </c>
+      <c r="J2" s="5">
+        <v>1</v>
+      </c>
+      <c r="K2" s="5">
         <v>1100</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="5">
         <v>1920</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="5">
         <f>K2*279</f>
         <v>306900</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="O2" t="b">
-        <v>0</v>
-      </c>
-      <c r="P2">
+      <c r="O2" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="P2" s="5">
         <v>-90.296126999999998</v>
       </c>
-      <c r="Q2">
+      <c r="Q2" s="5">
         <v>43.224344000000002</v>
       </c>
-      <c r="R2">
+      <c r="R2" s="5">
         <v>700</v>
       </c>
     </row>
@@ -2019,60 +2049,60 @@
         <v>700</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="5">
         <v>100000000</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="5">
         <v>100000000</v>
       </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="D6" s="5">
+        <v>1</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="6">
         <f t="shared" si="0"/>
         <v>1449.4183821327754</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
-      <c r="J6">
-        <v>1</v>
-      </c>
-      <c r="K6">
+      <c r="I6" s="5">
+        <v>1</v>
+      </c>
+      <c r="J6" s="5">
+        <v>1</v>
+      </c>
+      <c r="K6" s="5">
         <v>1100</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="5">
         <v>1920</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="5">
         <v>300000</v>
       </c>
-      <c r="N6" t="s">
+      <c r="N6" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="O6" t="b">
-        <v>1</v>
-      </c>
-      <c r="P6">
+      <c r="O6" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="P6" s="5">
         <v>-90.295053999999993</v>
       </c>
-      <c r="Q6">
+      <c r="Q6" s="5">
         <v>43.224375000000002</v>
       </c>
-      <c r="R6">
+      <c r="R6" s="5">
         <v>700</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Ensured recovery assistance calcs done w/ entity's original property
</commit_message>
<xml_diff>
--- a/inputs/desaster_input_data_template.xlsx
+++ b/inputs/desaster_input_data_template.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="renters" sheetId="5" r:id="rId1"/>
     <sheet name="owners" sheetId="1" r:id="rId2"/>
     <sheet name="forsale_stock" sheetId="2" r:id="rId3"/>
     <sheet name="forrent_stock" sheetId="6" r:id="rId4"/>
+    <sheet name="temp_stock" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -30,10 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="79">
-  <si>
-    <t>Savings</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="81">
   <si>
     <t>Address</t>
   </si>
@@ -41,9 +39,6 @@
     <t>Occupancy</t>
   </si>
   <si>
-    <t>Cost</t>
-  </si>
-  <si>
     <t>Bedrooms</t>
   </si>
   <si>
@@ -267,6 +262,18 @@
   </si>
   <si>
     <t>Blake</t>
+  </si>
+  <si>
+    <t>12300 Lodging Rd</t>
+  </si>
+  <si>
+    <t>Temporary Lodging</t>
+  </si>
+  <si>
+    <t>Hotel</t>
+  </si>
+  <si>
+    <t>Best Western</t>
   </si>
 </sst>
 </file>
@@ -305,7 +312,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -318,6 +325,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -328,7 +341,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="173">
+  <cellStyleXfs count="263">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -502,8 +515,98 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="38" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -513,8 +616,11 @@
     <xf numFmtId="38" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="38" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="173">
+  <cellStyles count="263">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -601,6 +707,51 @@
     <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -687,6 +838,51 @@
     <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -964,8 +1160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -975,84 +1171,84 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H1" t="s">
-        <v>66</v>
-      </c>
-      <c r="I1" t="s">
-        <v>68</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" t="s">
         <v>4</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>5</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>6</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>7</v>
       </c>
-      <c r="N1" t="s">
-        <v>8</v>
-      </c>
-      <c r="O1" t="s">
-        <v>9</v>
-      </c>
       <c r="P1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="Q1" t="s">
+        <v>58</v>
+      </c>
+      <c r="R1" t="s">
+        <v>41</v>
+      </c>
+      <c r="S1" t="s">
+        <v>53</v>
+      </c>
+      <c r="T1" t="s">
+        <v>59</v>
+      </c>
+      <c r="U1" t="s">
         <v>60</v>
       </c>
-      <c r="R1" t="s">
-        <v>43</v>
-      </c>
-      <c r="S1" t="s">
-        <v>55</v>
-      </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>61</v>
-      </c>
-      <c r="U1" t="s">
-        <v>62</v>
-      </c>
-      <c r="V1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E2">
         <f>12*I2/0.25</f>
@@ -1088,10 +1284,10 @@
         <v>279000</v>
       </c>
       <c r="O2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="P2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="Q2">
         <v>30000</v>
@@ -1114,16 +1310,16 @@
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E5" si="0">12*I3/0.25</f>
@@ -1159,10 +1355,10 @@
         <v>418500</v>
       </c>
       <c r="O3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="P3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="Q3">
         <v>30000</v>
@@ -1185,16 +1381,16 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E4">
         <v>1000000</v>
@@ -1229,10 +1425,10 @@
         <v>139500</v>
       </c>
       <c r="O4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="P4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="Q4">
         <v>30000</v>
@@ -1255,16 +1451,16 @@
     </row>
     <row r="5" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E5" s="8">
         <f t="shared" si="0"/>
@@ -1300,10 +1496,10 @@
         <v>558000</v>
       </c>
       <c r="O5" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="P5" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="Q5" s="8">
         <v>30000</v>
@@ -1326,16 +1522,16 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E6">
         <v>100000000</v>
@@ -1370,10 +1566,10 @@
         <v>279000</v>
       </c>
       <c r="O6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="P6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="Q6">
         <v>100000000</v>
@@ -1396,16 +1592,16 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E7">
         <v>100000000</v>
@@ -1440,10 +1636,10 @@
         <v>418500</v>
       </c>
       <c r="O7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="P7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="Q7">
         <v>100000000</v>
@@ -1466,16 +1662,16 @@
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E8">
         <v>100000000</v>
@@ -1510,10 +1706,10 @@
         <v>139500</v>
       </c>
       <c r="O8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="P8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="Q8">
         <v>100000000</v>
@@ -1536,16 +1732,16 @@
     </row>
     <row r="9" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E9" s="8">
         <v>100000000</v>
@@ -1580,10 +1776,10 @@
         <v>558000</v>
       </c>
       <c r="O9" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="P9" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="Q9" s="8">
         <v>100000000</v>
@@ -1606,16 +1802,16 @@
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E10">
         <v>60000</v>
@@ -1649,10 +1845,10 @@
         <v>306900</v>
       </c>
       <c r="O10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="P10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="Q10">
         <v>30000</v>
@@ -1675,16 +1871,16 @@
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E11" s="3">
         <v>60000</v>
@@ -1718,10 +1914,10 @@
         <v>209250</v>
       </c>
       <c r="O11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="P11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="Q11" s="3">
         <v>30000</v>
@@ -1752,8 +1948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1763,63 +1959,63 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O1" t="s">
+        <v>53</v>
+      </c>
+      <c r="P1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q1" t="s">
         <v>60</v>
       </c>
-      <c r="D1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" t="s">
-        <v>70</v>
-      </c>
-      <c r="I1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O1" t="s">
-        <v>55</v>
-      </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>61</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>62</v>
-      </c>
-      <c r="R1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B2" s="5">
         <v>60000</v>
@@ -1831,17 +2027,17 @@
         <v>0</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F2" s="6">
         <f>-PMT(0.05/12,360,(M2-M2*0.1),0)</f>
         <v>1482.7550049218294</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I2" s="5">
         <v>1</v>
@@ -1860,7 +2056,7 @@
         <v>306900</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O2" s="5" t="b">
         <v>0</v>
@@ -1877,7 +2073,7 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>1000000</v>
@@ -1889,17 +2085,17 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F3" s="2">
         <f t="shared" ref="F3:F9" si="0">-PMT(0.05/12,360,(M3-M3*0.1),0)</f>
         <v>4043.8772861504435</v>
       </c>
       <c r="G3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I3">
         <v>4</v>
@@ -1918,7 +2114,7 @@
         <v>837000</v>
       </c>
       <c r="N3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="O3" t="b">
         <v>0</v>
@@ -1935,7 +2131,7 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B4">
         <v>45000</v>
@@ -1947,17 +2143,17 @@
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F4" s="2">
         <f t="shared" si="0"/>
         <v>1010.9693215376109</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I4">
         <v>2</v>
@@ -1976,7 +2172,7 @@
         <v>209250</v>
       </c>
       <c r="N4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="O4" t="b">
         <v>0</v>
@@ -1993,7 +2189,7 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B5">
         <v>125000</v>
@@ -2005,17 +2201,17 @@
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F5" s="2">
         <f t="shared" si="0"/>
         <v>2695.9181907669627</v>
       </c>
       <c r="G5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I5">
         <v>3</v>
@@ -2034,7 +2230,7 @@
         <v>558000</v>
       </c>
       <c r="N5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="O5" t="b">
         <v>0</v>
@@ -2051,7 +2247,7 @@
     </row>
     <row r="6" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B6" s="5">
         <v>100000000</v>
@@ -2063,17 +2259,17 @@
         <v>1</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F6" s="6">
         <f t="shared" si="0"/>
         <v>1449.4183821327754</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I6" s="5">
         <v>1</v>
@@ -2091,7 +2287,7 @@
         <v>300000</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="O6" s="5" t="b">
         <v>1</v>
@@ -2108,7 +2304,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B7">
         <v>100000000</v>
@@ -2120,17 +2316,17 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F7" s="2">
         <f t="shared" si="0"/>
         <v>3865.1156856874013</v>
       </c>
       <c r="G7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I7">
         <v>4</v>
@@ -2148,7 +2344,7 @@
         <v>800000</v>
       </c>
       <c r="N7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="O7" t="b">
         <v>1</v>
@@ -2165,7 +2361,7 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B8">
         <v>100000000</v>
@@ -2177,17 +2373,17 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F8" s="2">
         <f t="shared" si="0"/>
         <v>1010.9693215376109</v>
       </c>
       <c r="G8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I8">
         <v>2</v>
@@ -2206,7 +2402,7 @@
         <v>209250</v>
       </c>
       <c r="N8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="O8" t="b">
         <v>1</v>
@@ -2223,7 +2419,7 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B9">
         <v>100000000</v>
@@ -2235,17 +2431,17 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F9" s="2">
         <f t="shared" si="0"/>
         <v>2415.6973035546257</v>
       </c>
       <c r="G9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I9">
         <v>3</v>
@@ -2263,7 +2459,7 @@
         <v>500000</v>
       </c>
       <c r="N9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="O9" t="b">
         <v>1</v>
@@ -2286,232 +2482,516 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:N5"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="K1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="9">
+        <v>60000</v>
+      </c>
+      <c r="C2" s="9">
+        <v>100000</v>
+      </c>
+      <c r="D2" s="9">
+        <v>0</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="10">
+        <v>1483</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="I2" s="9">
+        <v>1</v>
+      </c>
+      <c r="J2" s="9">
+        <v>1</v>
+      </c>
+      <c r="K2" s="9">
+        <v>1100</v>
+      </c>
+      <c r="L2" s="9">
+        <v>1920</v>
+      </c>
+      <c r="M2" s="9">
+        <v>306900</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="O2" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="P2" s="9">
+        <v>-90.296126999999998</v>
+      </c>
+      <c r="Q2" s="9">
+        <v>43.224344000000002</v>
+      </c>
+      <c r="R2" s="9">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="C3" s="3">
+        <v>100</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="4">
+        <v>4044</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I3" s="3">
+        <v>4</v>
+      </c>
+      <c r="J3" s="3">
+        <v>3</v>
+      </c>
+      <c r="K3" s="3">
+        <v>3000</v>
+      </c>
+      <c r="L3" s="3">
+        <v>1920</v>
+      </c>
+      <c r="M3" s="3">
+        <v>837000</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="O3" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="P3" s="3">
+        <v>-90.295697000000004</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>43.224218999999998</v>
+      </c>
+      <c r="R3" s="3">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="3">
+        <v>45000</v>
+      </c>
+      <c r="C4" s="3">
+        <v>50000</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="4">
+        <v>1011</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I4" s="3">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J4" s="3">
+        <v>1</v>
+      </c>
+      <c r="K4" s="3">
+        <v>750</v>
+      </c>
+      <c r="L4" s="3">
+        <v>1960</v>
+      </c>
+      <c r="M4" s="3">
+        <v>209250</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="O4" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="P4" s="3">
+        <v>-90.296706</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>43.223984000000002</v>
+      </c>
+      <c r="R4" s="3">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="3">
+        <v>125000</v>
+      </c>
+      <c r="C5" s="3">
+        <v>100</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="4">
+        <v>2696</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I5" s="3">
+        <v>3</v>
+      </c>
+      <c r="J5" s="3">
+        <v>2</v>
+      </c>
+      <c r="K5" s="3">
+        <v>2000</v>
+      </c>
+      <c r="L5" s="3">
+        <v>2010</v>
+      </c>
+      <c r="M5" s="3">
+        <v>558000</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="O5" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="P5" s="3">
+        <v>-90.296642000000006</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>43.223750000000003</v>
+      </c>
+      <c r="R5" s="3">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="9">
+        <v>100000000</v>
+      </c>
+      <c r="C6" s="9">
+        <v>100000000</v>
+      </c>
+      <c r="D6" s="9">
+        <v>1</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="10">
+        <v>1449</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="I6" s="9">
+        <v>1</v>
+      </c>
+      <c r="J6" s="9">
+        <v>1</v>
+      </c>
+      <c r="K6" s="9">
+        <v>1100</v>
+      </c>
+      <c r="L6" s="9">
+        <v>1920</v>
+      </c>
+      <c r="M6" s="9">
+        <v>300000</v>
+      </c>
+      <c r="N6" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="O6" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="P6" s="9">
+        <v>-90.295053999999993</v>
+      </c>
+      <c r="Q6" s="9">
+        <v>43.224375000000002</v>
+      </c>
+      <c r="R6" s="9">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="3">
+        <v>100000000</v>
+      </c>
+      <c r="C7" s="3">
+        <v>100000000</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="4">
+        <v>3865</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I7" s="3">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" t="s">
-        <v>61</v>
-      </c>
-      <c r="N1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="J7" s="3">
+        <v>3</v>
+      </c>
+      <c r="K7" s="3">
+        <v>3000</v>
+      </c>
+      <c r="L7" s="3">
+        <v>1920</v>
+      </c>
+      <c r="M7" s="3">
+        <v>800000</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="O7" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="P7" s="3">
+        <v>-90.294539</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>43.224390999999997</v>
+      </c>
+      <c r="R7" s="3">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="3">
+        <v>100000000</v>
+      </c>
+      <c r="C8" s="3">
+        <v>100000000</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="4">
+        <v>1011</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I8" s="3">
+        <v>2</v>
+      </c>
+      <c r="J8" s="3">
+        <v>1</v>
+      </c>
+      <c r="K8" s="3">
+        <v>750</v>
+      </c>
+      <c r="L8" s="3">
+        <v>1960</v>
+      </c>
+      <c r="M8" s="3">
+        <v>209250</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="O8" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="P8" s="3">
+        <v>-90.295225000000002</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>43.223953000000002</v>
+      </c>
+      <c r="R8" s="3">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B2">
+      <c r="B9" s="3">
         <v>100000000</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2">
-        <v>1000</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>1100</v>
-      </c>
-      <c r="J2">
-        <v>1920</v>
-      </c>
-      <c r="K2">
-        <v>100000</v>
-      </c>
-      <c r="L2" t="s">
-        <v>44</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3">
+      <c r="C9" s="3">
         <v>100000000</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="D9" s="3">
+        <v>1</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E3">
-        <v>4000</v>
-      </c>
-      <c r="F3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3">
-        <v>4</v>
-      </c>
-      <c r="H3">
-        <v>5</v>
-      </c>
-      <c r="I3">
-        <v>5000</v>
-      </c>
-      <c r="J3">
-        <v>1920</v>
-      </c>
-      <c r="K3">
-        <v>10000000</v>
-      </c>
-      <c r="L3" t="s">
-        <v>46</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B4">
-        <v>100000000</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4">
-        <v>1000</v>
-      </c>
-      <c r="F4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4">
+      <c r="F9" s="4">
+        <v>2416</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I9" s="3">
+        <v>3</v>
+      </c>
+      <c r="J9" s="3">
         <v>2</v>
       </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <v>1200</v>
-      </c>
-      <c r="J4">
-        <v>1960</v>
-      </c>
-      <c r="K4">
-        <v>10000</v>
-      </c>
-      <c r="L4" t="s">
-        <v>45</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B5">
-        <v>100000000</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5">
+      <c r="K9" s="3">
         <v>2000</v>
       </c>
-      <c r="F5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5">
-        <v>3</v>
-      </c>
-      <c r="H5">
-        <v>2</v>
-      </c>
-      <c r="I5">
-        <v>2000</v>
-      </c>
-      <c r="J5">
+      <c r="L9" s="3">
         <v>2010</v>
       </c>
-      <c r="K5">
-        <v>800000</v>
-      </c>
-      <c r="L5" t="s">
-        <v>18</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5">
-        <v>0</v>
+      <c r="M9" s="3">
+        <v>500000</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="O9" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="P9" s="3">
+        <v>-90.295225000000002</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>43.223717999999998</v>
+      </c>
+      <c r="R9" s="3">
+        <v>700</v>
       </c>
     </row>
   </sheetData>
@@ -2521,26 +3001,29 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:V7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="10" max="10" width="16.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>66</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -2561,195 +3044,719 @@
         <v>7</v>
       </c>
       <c r="K1" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="L1" t="s">
-        <v>9</v>
+        <v>58</v>
       </c>
       <c r="M1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N1" t="s">
+        <v>53</v>
+      </c>
+      <c r="O1" t="s">
+        <v>59</v>
+      </c>
+      <c r="P1" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q1" t="s">
         <v>61</v>
       </c>
-      <c r="N1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2">
+        <v>48</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2">
         <v>100000000</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="F2">
+        <v>1000</v>
+      </c>
+      <c r="G2">
+        <v>700</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <f>2.48*L2</f>
+        <v>2480</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1000</v>
+      </c>
+      <c r="M2">
+        <v>1920</v>
+      </c>
+      <c r="N2">
+        <f>279*L2</f>
+        <v>279000</v>
+      </c>
+      <c r="O2" t="s">
+        <v>65</v>
+      </c>
+      <c r="P2" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q2">
+        <v>100000000</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2" t="b">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>-90.293080000000003</v>
+      </c>
+      <c r="U2">
+        <v>43.223671000000003</v>
+      </c>
+      <c r="V2">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3">
+        <v>100000000</v>
+      </c>
+      <c r="F3">
+        <v>1000</v>
+      </c>
+      <c r="G3">
+        <v>700</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I5" si="0">2.48*L3</f>
+        <v>3720</v>
+      </c>
+      <c r="J3">
+        <v>3</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+      <c r="L3">
+        <v>1500</v>
+      </c>
+      <c r="M3">
+        <v>1920</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N5" si="1">279*L3</f>
+        <v>418500</v>
+      </c>
+      <c r="O3" t="s">
+        <v>65</v>
+      </c>
+      <c r="P3" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q3">
+        <v>100000000</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3" t="b">
+        <v>1</v>
+      </c>
+      <c r="T3">
+        <v>-90.292736000000005</v>
+      </c>
+      <c r="U3">
+        <v>43.223545999999999</v>
+      </c>
+      <c r="V3">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" t="s">
         <v>34</v>
       </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2">
-        <v>100</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>700</v>
-      </c>
-      <c r="J2">
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4">
+        <v>100000000</v>
+      </c>
+      <c r="F4">
+        <v>1000</v>
+      </c>
+      <c r="G4">
+        <v>700</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>1240</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>500</v>
+      </c>
+      <c r="M4">
+        <v>1960</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="1"/>
+        <v>139500</v>
+      </c>
+      <c r="O4" t="s">
+        <v>65</v>
+      </c>
+      <c r="P4" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q4">
+        <v>100000000</v>
+      </c>
+      <c r="R4">
+        <v>1</v>
+      </c>
+      <c r="S4" t="b">
+        <v>1</v>
+      </c>
+      <c r="T4">
+        <v>-90.296190999999993</v>
+      </c>
+      <c r="U4">
+        <v>43.223405999999997</v>
+      </c>
+      <c r="V4">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="E5" s="8">
+        <v>100000000</v>
+      </c>
+      <c r="F5" s="8">
+        <v>1000</v>
+      </c>
+      <c r="G5" s="8">
+        <v>700</v>
+      </c>
+      <c r="H5" s="8">
+        <v>0</v>
+      </c>
+      <c r="I5" s="8">
+        <f t="shared" si="0"/>
+        <v>4960</v>
+      </c>
+      <c r="J5" s="8">
+        <v>2</v>
+      </c>
+      <c r="K5" s="8">
+        <v>2</v>
+      </c>
+      <c r="L5" s="8">
+        <v>2000</v>
+      </c>
+      <c r="M5" s="8">
+        <v>2010</v>
+      </c>
+      <c r="N5" s="8">
+        <f t="shared" si="1"/>
+        <v>558000</v>
+      </c>
+      <c r="O5" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="P5" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q5" s="8">
+        <v>100000000</v>
+      </c>
+      <c r="R5" s="8">
+        <v>1</v>
+      </c>
+      <c r="S5" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="T5" s="8">
+        <v>-90.295739999999995</v>
+      </c>
+      <c r="U5" s="8">
+        <v>43.223359000000002</v>
+      </c>
+      <c r="V5" s="8">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E6">
+        <v>60000</v>
+      </c>
+      <c r="F6">
+        <v>1000</v>
+      </c>
+      <c r="G6">
+        <v>700</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>1100</v>
+      </c>
+      <c r="M6">
         <v>1920</v>
       </c>
-      <c r="K2">
-        <v>99999</v>
-      </c>
-      <c r="L2" t="s">
-        <v>18</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3">
-        <v>100000000</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3">
-        <v>100000</v>
-      </c>
-      <c r="G3">
+      <c r="N6">
+        <f>L6*279</f>
+        <v>306900</v>
+      </c>
+      <c r="O6" t="s">
+        <v>65</v>
+      </c>
+      <c r="P6" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q6">
+        <v>30000</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6" t="b">
+        <v>1</v>
+      </c>
+      <c r="T6">
+        <v>-90.294238000000007</v>
+      </c>
+      <c r="U6">
+        <v>43.224015000000001</v>
+      </c>
+      <c r="V6">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" s="3">
+        <v>60000</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1000</v>
+      </c>
+      <c r="G7" s="3">
+        <v>700</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0</v>
+      </c>
+      <c r="I7" s="4">
+        <v>1</v>
+      </c>
+      <c r="J7">
         <v>2</v>
       </c>
-      <c r="H3">
-        <v>2</v>
-      </c>
-      <c r="I3">
-        <v>5000</v>
-      </c>
-      <c r="J3">
-        <v>1920</v>
-      </c>
-      <c r="K3">
-        <v>9999</v>
-      </c>
-      <c r="L3" t="s">
-        <v>18</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B4">
-        <v>100000000</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4">
-        <v>10</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <v>250</v>
-      </c>
-      <c r="J4">
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>750</v>
+      </c>
+      <c r="M7">
         <v>1960</v>
       </c>
-      <c r="K4">
-        <v>9999</v>
-      </c>
-      <c r="L4" t="s">
-        <v>18</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5">
-        <v>100000000</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5">
-        <v>2000</v>
-      </c>
-      <c r="G5">
-        <v>3</v>
-      </c>
-      <c r="H5">
-        <v>2</v>
-      </c>
-      <c r="I5">
-        <v>2000</v>
-      </c>
-      <c r="J5">
-        <v>2010</v>
-      </c>
-      <c r="K5">
-        <v>800000</v>
-      </c>
-      <c r="L5" t="s">
-        <v>18</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5">
-        <v>0</v>
+      <c r="N7">
+        <f t="shared" ref="N7" si="2">L7*279</f>
+        <v>209250</v>
+      </c>
+      <c r="O7" t="s">
+        <v>65</v>
+      </c>
+      <c r="P7" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>30000</v>
+      </c>
+      <c r="R7" s="3">
+        <v>0</v>
+      </c>
+      <c r="S7" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="T7" s="3">
+        <v>-90.294238000000007</v>
+      </c>
+      <c r="U7" s="3">
+        <v>43.224015000000001</v>
+      </c>
+      <c r="V7" s="3">
+        <v>700</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="10" max="10" width="16.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L1" t="s">
+        <v>58</v>
+      </c>
+      <c r="M1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N1" t="s">
+        <v>53</v>
+      </c>
+      <c r="O1" t="s">
+        <v>59</v>
+      </c>
+      <c r="P1" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2">
+        <v>3000</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>500</v>
+      </c>
+      <c r="H2">
+        <v>1990</v>
+      </c>
+      <c r="J2" t="s">
+        <v>65</v>
+      </c>
+      <c r="K2" t="s">
+        <v>80</v>
+      </c>
+      <c r="L2">
+        <v>10000000</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2" t="b">
+        <v>1</v>
+      </c>
+      <c r="O2" s="3">
+        <v>-90.294238000000007</v>
+      </c>
+      <c r="P2" s="3">
+        <v>43.224015000000001</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3">
+        <v>4000</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>500</v>
+      </c>
+      <c r="H3">
+        <v>1990</v>
+      </c>
+      <c r="J3" t="s">
+        <v>65</v>
+      </c>
+      <c r="K3" t="s">
+        <v>80</v>
+      </c>
+      <c r="L3">
+        <v>10000000</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3" t="b">
+        <v>1</v>
+      </c>
+      <c r="O3" s="3">
+        <v>-90.294238000000007</v>
+      </c>
+      <c r="P3" s="3">
+        <v>43.224015000000001</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4">
+        <v>5000</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>500</v>
+      </c>
+      <c r="H4">
+        <v>1990</v>
+      </c>
+      <c r="J4" t="s">
+        <v>65</v>
+      </c>
+      <c r="K4" t="s">
+        <v>80</v>
+      </c>
+      <c r="L4">
+        <v>10000000</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O4" s="3">
+        <v>-90.294238000000007</v>
+      </c>
+      <c r="P4" s="3">
+        <v>43.224015000000001</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5">
+        <v>6000</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>500</v>
+      </c>
+      <c r="H5">
+        <v>1990</v>
+      </c>
+      <c r="J5" t="s">
+        <v>65</v>
+      </c>
+      <c r="K5" t="s">
+        <v>80</v>
+      </c>
+      <c r="L5">
+        <v>10000000</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5" t="b">
+        <v>1</v>
+      </c>
+      <c r="O5" s="3">
+        <v>-90.294238000000007</v>
+      </c>
+      <c r="P5" s="3">
+        <v>43.224015000000001</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>700</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>